<commit_message>
test: add other answer test
</commit_message>
<xml_diff>
--- a/tests/answer/case/estimation-other.test-cases.xlsx
+++ b/tests/answer/case/estimation-other.test-cases.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/cfp-calc/tests/answer/case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5C8C9-13FC-414E-B7C2-493359AF5F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9743099-A751-9C46-9A50-01A0C622AAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="10" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="51200" yWindow="5300" windowWidth="38400" windowHeight="23500" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="answers" sheetId="1" r:id="rId1"/>
+    <sheet name="answers" sheetId="23" r:id="rId1"/>
     <sheet name="otherE1" sheetId="15" r:id="rId2"/>
     <sheet name="otherE2" sheetId="17" r:id="rId3"/>
     <sheet name="otherE3" sheetId="18" r:id="rId4"/>
@@ -1891,7 +1891,7 @@
         <xdr:cNvPr id="2" name="テキスト ボックス 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD164EB-5EDA-EEC2-247A-59C8CF9B2EA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59B1CAA8-CD9B-BE4A-87A0-CB269B8A3D73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1899,7 +1899,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8864600" y="2476500"/>
+          <a:off x="7912100" y="9588500"/>
           <a:ext cx="8105873" cy="3530069"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2115,10 +2115,10 @@
     <xdr:ext cx="5892800" cy="564257"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="テキスト ボックス 3">
+        <xdr:cNvPr id="3" name="テキスト ボックス 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E82A8FD-CF92-AA47-BC53-A02669A0C84B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22F76B35-0F59-A14B-BD23-70AD228BBC7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2494,14 +2494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D200101-8AE2-B047-8D74-11158EABAA81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CC585B-0CCC-A944-8580-30969A5D6B8C}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -6438,7 +6438,7 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>